<commit_message>
reading more KOP tweets
</commit_message>
<xml_diff>
--- a/KOP brexit.xlsx
+++ b/KOP brexit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roy\Documents\A IDC Roy BDA\Third Year - BDA\Semester 2\סטאז'\code new\brexit-package-new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B845E4B-0E32-4128-91A7-1180201BD6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BF550D-7591-4EBE-8990-434E94E4BDBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KOP brexit" sheetId="1" r:id="rId1"/>
@@ -910,7 +910,31 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCE5CD"/>
+          <bgColor rgb="FFFCE5CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC9DAF8"/>
+          <bgColor rgb="FFC9DAF8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -962,9 +986,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="KOP brexit-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstRowStripe" dxfId="4"/>
-      <tableStyleElement type="secondRowStripe" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="secondRowStripe" dxfId="6"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1194,7 +1218,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F69" sqref="F69"/>
+      <selection pane="bottomLeft" activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2619,7 +2643,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="7">
         <v>63</v>
       </c>
@@ -2634,7 +2658,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="7">
         <v>64</v>
       </c>
@@ -2649,7 +2673,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="7">
         <v>65</v>
       </c>
@@ -2664,7 +2688,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="7">
         <v>66</v>
       </c>
@@ -2679,7 +2703,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="8">
         <v>67</v>
       </c>
@@ -2694,7 +2718,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="8">
         <v>68</v>
       </c>
@@ -2709,7 +2733,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="7">
         <v>69</v>
       </c>
@@ -2724,7 +2748,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="7">
         <v>70</v>
       </c>
@@ -2737,7 +2761,7 @@
       </c>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="7">
         <v>71</v>
       </c>
@@ -2752,7 +2776,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="7">
         <v>72</v>
       </c>
@@ -2765,22 +2789,30 @@
       </c>
       <c r="E74" s="7"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+    </row>
+    <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B78" s="1"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B79" s="1"/>
     </row>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B80" s="1"/>
     </row>
     <row r="81" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5535,19 +5567,34 @@
       <c r="B997" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B997">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="1">
+  <conditionalFormatting sqref="B1:B74 B76:B997">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH(("1"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B997">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="2">
+  <conditionalFormatting sqref="B1:B74 B76:B997">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH(("2"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B997">
+  <conditionalFormatting sqref="B1:B74 B76:B997">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="3">
+      <formula>NOT(ISERROR(SEARCH(("3"),(B1))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH(("1"),(B75))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="2">
+      <formula>NOT(ISERROR(SEARCH(("2"),(B75))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75">
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="3">
-      <formula>NOT(ISERROR(SEARCH(("3"),(B1))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("3"),(B75))))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>

</xml_diff>